<commit_message>
new file:   .gitignore 	new file:   __init__.py 	new file:   event_calendar.py 	new file:   event_items.py 	modified:   "\345\244\251\345\234\260\345\274\210\345\261\200.py" 	modified:   "\346\264\273\345\212\250\346\227\245\345\216\206.xlsx" 	deleted:    "\347\245\236\347\211\251\345\233\255.py" 	modified:   "\350\231\232\345\244\251\346\256\277.py"
</commit_message>
<xml_diff>
--- a/活动日历.xlsx
+++ b/活动日历.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\科学修仙\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7D3A7C-5ED0-4EA6-8669-670350CBF1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C8BD37-B27A-4902-8533-0615D409A8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7414" yWindow="2940" windowWidth="24686" windowHeight="13054" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,40 +26,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>event</t>
-  </si>
-  <si>
     <t>虚天殿跨服2</t>
   </si>
   <si>
-    <t>虚天殿跨服2, 灵宠竞武</t>
-  </si>
-  <si>
-    <t>灵宠竞武, 天地弈局</t>
-  </si>
-  <si>
-    <t>天地弈局跨服4, 瑶池花会跨服2</t>
-  </si>
-  <si>
-    <t>瑶池花会跨服2, 兽渊探秘跨服2</t>
-  </si>
-  <si>
-    <t>兽渊探秘跨服2, 丹道问鼎跨服2</t>
-  </si>
-  <si>
-    <t>丹道问鼎跨服2, 升仙会跨服2</t>
+    <t>灵宠竞武</t>
+  </si>
+  <si>
+    <t>天地弈局</t>
+  </si>
+  <si>
+    <t>瑶池花会跨服2</t>
+  </si>
+  <si>
+    <t>兽渊探秘跨服2</t>
+  </si>
+  <si>
+    <t>丹道问鼎跨服2</t>
+  </si>
+  <si>
+    <t>升仙会跨服2</t>
+  </si>
+  <si>
+    <t>云梦试剑跨服2</t>
+  </si>
+  <si>
+    <t>魔道入侵</t>
+  </si>
+  <si>
+    <t>炼体法相预赛</t>
+  </si>
+  <si>
+    <t>天地弈局跨服4</t>
+  </si>
+  <si>
+    <t>魔道入侵预赛</t>
+  </si>
+  <si>
+    <t>天地弈局预赛</t>
+  </si>
+  <si>
+    <t>虚天殿</t>
+  </si>
+  <si>
+    <t>云梦试剑</t>
+  </si>
+  <si>
+    <t>兽渊</t>
+  </si>
+  <si>
+    <t>丹道问鼎</t>
+  </si>
+  <si>
+    <t>炼体法相</t>
+  </si>
+  <si>
+    <t>瑶池花会</t>
+  </si>
+  <si>
+    <t>服内</t>
+  </si>
+  <si>
+    <t>2跨</t>
+  </si>
+  <si>
+    <t>4跨</t>
+  </si>
+  <si>
+    <t>8跨</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,16 +115,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,13 +145,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,88 +482,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.15234375" customWidth="1"/>
+    <col min="1" max="1" width="13.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.4609375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" style="1"/>
+    <col min="4" max="4" width="15.4609375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="2">
+        <v>45164</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="2">
+        <v>45165</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="2">
+        <v>45166</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>45167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="2">
+        <v>45168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>45169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="2">
+        <v>45171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="2">
+        <v>45172</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078B6838-5F0B-42EF-8CED-D0169CE431F7}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="8" width="10.07421875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="10.07421875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.23046875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="6">
         <v>45164</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" s="6">
+        <v>45165</v>
+      </c>
+      <c r="C1" s="6">
+        <v>45166</v>
+      </c>
+      <c r="D1" s="6">
+        <v>45167</v>
+      </c>
+      <c r="E1" s="6">
+        <v>45168</v>
+      </c>
+      <c r="F1" s="6">
+        <v>45169</v>
+      </c>
+      <c r="G1" s="6">
+        <v>45170</v>
+      </c>
+      <c r="H1" s="6">
+        <v>45171</v>
+      </c>
+      <c r="I1" s="6">
+        <v>45172</v>
+      </c>
+      <c r="J1" s="6">
+        <v>45173</v>
+      </c>
+      <c r="K1" s="6">
+        <v>45174</v>
+      </c>
+      <c r="L1" s="6">
+        <v>45175</v>
+      </c>
+      <c r="M1" s="6">
+        <v>45176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="45.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="8"/>
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
-        <v>45165</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
-        <v>45166</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
-        <v>45167</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5">
+        <v>-2</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
-        <v>45168</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
-        <v>45169</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="1">
-        <v>45170</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" s="1">
-        <v>45171</v>
-      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5">
+        <v>-1</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>